<commit_message>
minor bug fixes in get_pf_shortcircuit_results.py; edited load_pf_results in test_all_faults_and_cases.py
</commit_message>
<xml_diff>
--- a/pandapower/test/shortcircuit/SCE_Tests/sc_result_comparison/test_case_1_four_bus_radial_grid_pf_sc_results_branch.xlsx
+++ b/pandapower/test/shortcircuit/SCE_Tests/sc_result_comparison/test_case_1_four_bus_radial_grid_pf_sc_results_branch.xlsx
@@ -80,10 +80,10 @@
     <t>pf_q_to_mvar</t>
   </si>
   <si>
-    <t>pf_ikss_from_deg</t>
+    <t>pf_ikss_from_degree</t>
   </si>
   <si>
-    <t>pf_ikss_to_deg</t>
+    <t>pf_ikss_to_degree</t>
   </si>
   <si>
     <t>pf_vm_from_pu</t>
@@ -92,10 +92,10 @@
     <t>pf_vm_to_pu</t>
   </si>
   <si>
-    <t>pf_va_from_deg</t>
+    <t>pf_va_from_degree</t>
   </si>
   <si>
-    <t>pf_va_to_deg</t>
+    <t>pf_va_to_degree</t>
   </si>
   <si>
     <t>Line_0</t>
@@ -161,76 +161,76 @@
     <t>pf_p_c_to_mw</t>
   </si>
   <si>
-    <t>pf_q_a_from_mw</t>
+    <t>pf_q_a_from_mvar</t>
   </si>
   <si>
-    <t>pf_q_b_from_mw</t>
+    <t>pf_q_b_from_mvar</t>
   </si>
   <si>
-    <t>pf_q_c_from_mw</t>
+    <t>pf_q_c_from_mvar</t>
   </si>
   <si>
-    <t>pf_q_a_to_mw</t>
+    <t>pf_q_a_to_mvar</t>
   </si>
   <si>
-    <t>pf_q_b_to_mw</t>
+    <t>pf_q_b_to_mvar</t>
   </si>
   <si>
-    <t>pf_q_c_to_mw</t>
+    <t>pf_q_c_to_mvar</t>
   </si>
   <si>
-    <t>pf_ikss_a_from_deg</t>
+    <t>pf_ikss_a_from_degree</t>
   </si>
   <si>
-    <t>pf_ikss_b_from_deg</t>
+    <t>pf_ikss_b_from_degree</t>
   </si>
   <si>
-    <t>pf_ikss_c_from_deg</t>
+    <t>pf_ikss_c_from_degree</t>
   </si>
   <si>
-    <t>pf_ikss_a_to_deg</t>
+    <t>pf_ikss_a_to_degree</t>
   </si>
   <si>
-    <t>pf_ikss_b_to_deg</t>
+    <t>pf_ikss_b_to_degree</t>
   </si>
   <si>
-    <t>pf_ikss_c_to_deg</t>
+    <t>pf_ikss_c_to_degree</t>
   </si>
   <si>
     <t>pf_vm_a_from_pu</t>
   </si>
   <si>
-    <t>pf_vm_b_from_bus_pu</t>
+    <t>pf_vm_b_from_pu</t>
   </si>
   <si>
-    <t>pf_vm_c_from_bus_pu</t>
+    <t>pf_vm_c_from_pu</t>
   </si>
   <si>
-    <t>pf_vm_a_to_bus_pu</t>
+    <t>pf_vm_a_to_pu</t>
   </si>
   <si>
-    <t>pf_vm_b_to_bus_pu</t>
+    <t>pf_vm_b_to_pu</t>
   </si>
   <si>
-    <t>pf_vm_c_to_bus_pu</t>
+    <t>pf_vm_c_to_pu</t>
   </si>
   <si>
-    <t>pf_va_a_from_bus_deg</t>
+    <t>pf_va_a_from_degree</t>
   </si>
   <si>
-    <t>pf_va_b_from_bus_deg</t>
+    <t>pf_va_b_from_degree</t>
   </si>
   <si>
-    <t>pf_va_c_from_bus_deg</t>
+    <t>pf_va_c_from_degree</t>
   </si>
   <si>
-    <t>pf_va_a_to_bus_deg</t>
+    <t>pf_va_a_to_degree</t>
   </si>
   <si>
-    <t>pf_va_b_to_bus_deg</t>
+    <t>pf_va_b_to_degree</t>
   </si>
   <si>
-    <t>pf_va_c_to_bus_deg</t>
+    <t>pf_va_c_to_degree</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
fixed va_degree export in get_pf_shortcircuit_results.py
</commit_message>
<xml_diff>
--- a/pandapower/test/shortcircuit/SCE_Tests/sc_result_comparison/test_case_1_four_bus_radial_grid_pf_sc_results_branch.xlsx
+++ b/pandapower/test/shortcircuit/SCE_Tests/sc_result_comparison/test_case_1_four_bus_radial_grid_pf_sc_results_branch.xlsx
@@ -694,10 +694,10 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>84.28940675037381</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>79.08778074434936</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -747,10 +747,10 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>79.08778074434936</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>75.11055707408345</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -800,10 +800,10 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>79.08778074434936</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>75.11055707408345</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1063,22 +1063,22 @@
         <v>0.952627964809529</v>
       </c>
       <c r="AL2">
-        <v>-6.289991047015337E-13</v>
+        <v>7.393038743051484E-13</v>
       </c>
       <c r="AM2">
-        <v>0</v>
+        <v>179.9999999999893</v>
       </c>
       <c r="AN2">
-        <v>179.9999999999919</v>
+        <v>179.9999999999889</v>
       </c>
       <c r="AO2">
-        <v>-4.852401742958505E-13</v>
+        <v>6.542352883650259E-13</v>
       </c>
       <c r="AP2">
-        <v>0</v>
+        <v>179.9999999999899</v>
       </c>
       <c r="AQ2">
-        <v>179.999999999992</v>
+        <v>179.9999999999892</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -1194,22 +1194,22 @@
         <v>0.9526279648097039</v>
       </c>
       <c r="AL3">
-        <v>-4.852401742958505E-13</v>
+        <v>6.542352883650259E-13</v>
       </c>
       <c r="AM3">
-        <v>0</v>
+        <v>179.9999999999899</v>
       </c>
       <c r="AN3">
-        <v>179.999999999992</v>
+        <v>179.9999999999892</v>
       </c>
       <c r="AO3">
-        <v>-3.643686092319228E-13</v>
+        <v>5.868810935265246E-13</v>
       </c>
       <c r="AP3">
-        <v>0</v>
+        <v>179.9999999999904</v>
       </c>
       <c r="AQ3">
-        <v>179.999999999992</v>
+        <v>179.9999999999894</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -1325,22 +1325,22 @@
         <v>0.9526279648097039</v>
       </c>
       <c r="AL4">
-        <v>-4.852401742958505E-13</v>
+        <v>6.542352883650259E-13</v>
       </c>
       <c r="AM4">
-        <v>0</v>
+        <v>179.9999999999899</v>
       </c>
       <c r="AN4">
-        <v>179.999999999992</v>
+        <v>179.9999999999892</v>
       </c>
       <c r="AO4">
-        <v>-3.588354961759716E-13</v>
+        <v>5.720494568375048E-13</v>
       </c>
       <c r="AP4">
-        <v>0</v>
+        <v>179.9999999999905</v>
       </c>
       <c r="AQ4">
-        <v>179.999999999992</v>
+        <v>179.9999999999895</v>
       </c>
     </row>
   </sheetData>
@@ -1600,22 +1600,22 @@
         <v>0.8990062051130553</v>
       </c>
       <c r="AL2">
-        <v>12.94734958163789</v>
+        <v>4.107243746137125E-13</v>
       </c>
       <c r="AM2">
-        <v>-111.8715959987214</v>
+        <v>-149.790502369296</v>
       </c>
       <c r="AN2">
-        <v>164.2547774324403</v>
+        <v>132.4483367722449</v>
       </c>
       <c r="AO2">
-        <v>12.10694022610787</v>
+        <v>3.729844236250756E-13</v>
       </c>
       <c r="AP2">
-        <v>-110.1555053571849</v>
+        <v>-150.9270159887323</v>
       </c>
       <c r="AQ2">
-        <v>165.7159849577473</v>
+        <v>136.7907349337361</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -1731,22 +1731,22 @@
         <v>0.9066188243642738</v>
       </c>
       <c r="AL3">
-        <v>12.10694022610787</v>
+        <v>3.729844236250756E-13</v>
       </c>
       <c r="AM3">
-        <v>-110.1555053571849</v>
+        <v>-150.9270159887323</v>
       </c>
       <c r="AN3">
-        <v>165.7159849577473</v>
+        <v>136.7907349337361</v>
       </c>
       <c r="AO3">
-        <v>11.33736026907989</v>
+        <v>3.432500056227896E-13</v>
       </c>
       <c r="AP3">
-        <v>-108.7272990406495</v>
+        <v>-152.098303223136</v>
       </c>
       <c r="AQ3">
-        <v>166.9361473250955</v>
+        <v>140.4399803555035</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -1862,22 +1862,22 @@
         <v>0.9066188243642738</v>
       </c>
       <c r="AL4">
-        <v>12.10694022610787</v>
+        <v>3.729844236250756E-13</v>
       </c>
       <c r="AM4">
-        <v>-110.1555053571849</v>
+        <v>-150.9270159887323</v>
       </c>
       <c r="AN4">
-        <v>165.7159849577473</v>
+        <v>136.7907349337361</v>
       </c>
       <c r="AO4">
-        <v>11.33736026907991</v>
+        <v>3.375329757114697E-13</v>
       </c>
       <c r="AP4">
-        <v>-108.7272990406495</v>
+        <v>-152.0983032231359</v>
       </c>
       <c r="AQ4">
-        <v>166.9361473250955</v>
+        <v>140.4399803555035</v>
       </c>
     </row>
   </sheetData>
@@ -2137,22 +2137,22 @@
         <v>0.8990062051130553</v>
       </c>
       <c r="AL2">
-        <v>12.94734958163789</v>
+        <v>4.107243746137125E-13</v>
       </c>
       <c r="AM2">
-        <v>-111.8715959987214</v>
+        <v>-149.790502369296</v>
       </c>
       <c r="AN2">
-        <v>164.2547774324403</v>
+        <v>132.4483367722449</v>
       </c>
       <c r="AO2">
-        <v>12.10694022610787</v>
+        <v>3.729844236250756E-13</v>
       </c>
       <c r="AP2">
-        <v>-110.1555053571849</v>
+        <v>-150.9270159887323</v>
       </c>
       <c r="AQ2">
-        <v>165.7159849577473</v>
+        <v>136.7907349337361</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -2268,22 +2268,22 @@
         <v>0.9066188243642738</v>
       </c>
       <c r="AL3">
-        <v>12.10694022610787</v>
+        <v>3.729844236250756E-13</v>
       </c>
       <c r="AM3">
-        <v>-110.1555053571849</v>
+        <v>-150.9270159887323</v>
       </c>
       <c r="AN3">
-        <v>165.7159849577473</v>
+        <v>136.7907349337361</v>
       </c>
       <c r="AO3">
-        <v>11.33736026907989</v>
+        <v>3.432500056227896E-13</v>
       </c>
       <c r="AP3">
-        <v>-108.7272990406495</v>
+        <v>-152.098303223136</v>
       </c>
       <c r="AQ3">
-        <v>166.9361473250955</v>
+        <v>140.4399803555035</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -2399,22 +2399,22 @@
         <v>0.9066188243642738</v>
       </c>
       <c r="AL4">
-        <v>12.10694022610787</v>
+        <v>3.729844236250756E-13</v>
       </c>
       <c r="AM4">
-        <v>-110.1555053571849</v>
+        <v>-150.9270159887323</v>
       </c>
       <c r="AN4">
-        <v>165.7159849577473</v>
+        <v>136.7907349337361</v>
       </c>
       <c r="AO4">
-        <v>11.33736026907991</v>
+        <v>3.375329757114697E-13</v>
       </c>
       <c r="AP4">
-        <v>-108.7272990406495</v>
+        <v>-152.0983032231359</v>
       </c>
       <c r="AQ4">
-        <v>166.9361473250955</v>
+        <v>140.4399803555035</v>
       </c>
     </row>
   </sheetData>
@@ -2674,22 +2674,22 @@
         <v>0.8660254037866308</v>
       </c>
       <c r="AL2">
-        <v>7.405398539844763E-12</v>
+        <v>6.886006733265022E-13</v>
       </c>
       <c r="AM2">
-        <v>0</v>
+        <v>-179.9999999999719</v>
       </c>
       <c r="AN2">
-        <v>179.9999999999839</v>
+        <v>179.9999999999648</v>
       </c>
       <c r="AO2">
-        <v>1.780692173543077E-11</v>
+        <v>5.344175747881745E-13</v>
       </c>
       <c r="AP2">
-        <v>0</v>
+        <v>-179.9999999999404</v>
       </c>
       <c r="AQ2">
-        <v>179.9999999999737</v>
+        <v>179.9999999999346</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -2805,22 +2805,22 @@
         <v>0.8660254037863299</v>
       </c>
       <c r="AL3">
-        <v>1.780692173543077E-11</v>
+        <v>5.344175747881745E-13</v>
       </c>
       <c r="AM3">
-        <v>0</v>
+        <v>-179.9999999999404</v>
       </c>
       <c r="AN3">
-        <v>179.9999999999737</v>
+        <v>179.9999999999346</v>
       </c>
       <c r="AO3">
-        <v>2.263570042986083E-11</v>
+        <v>4.559487397231727E-13</v>
       </c>
       <c r="AP3">
-        <v>0</v>
+        <v>-179.9999999999257</v>
       </c>
       <c r="AQ3">
-        <v>179.999999999969</v>
+        <v>179.9999999999208</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -2936,22 +2936,22 @@
         <v>0.8660254037863299</v>
       </c>
       <c r="AL4">
-        <v>1.780692173543077E-11</v>
+        <v>5.344175747881745E-13</v>
       </c>
       <c r="AM4">
-        <v>0</v>
+        <v>-179.9999999999404</v>
       </c>
       <c r="AN4">
-        <v>179.9999999999737</v>
+        <v>179.9999999999346</v>
       </c>
       <c r="AO4">
-        <v>2.263853053768626E-11</v>
+        <v>4.347494640096741E-13</v>
       </c>
       <c r="AP4">
-        <v>0</v>
+        <v>-179.9999999999256</v>
       </c>
       <c r="AQ4">
-        <v>179.999999999969</v>
+        <v>179.9999999999208</v>
       </c>
     </row>
   </sheetData>
@@ -3211,22 +3211,22 @@
         <v>0.8660254037866308</v>
       </c>
       <c r="AL2">
-        <v>7.405398539844763E-12</v>
+        <v>6.886006733265022E-13</v>
       </c>
       <c r="AM2">
-        <v>0</v>
+        <v>-179.9999999999719</v>
       </c>
       <c r="AN2">
-        <v>179.9999999999839</v>
+        <v>179.9999999999648</v>
       </c>
       <c r="AO2">
-        <v>1.780692173543077E-11</v>
+        <v>5.344175747881745E-13</v>
       </c>
       <c r="AP2">
-        <v>0</v>
+        <v>-179.9999999999404</v>
       </c>
       <c r="AQ2">
-        <v>179.9999999999737</v>
+        <v>179.9999999999346</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -3342,22 +3342,22 @@
         <v>0.8660254037863299</v>
       </c>
       <c r="AL3">
-        <v>1.780692173543077E-11</v>
+        <v>5.344175747881745E-13</v>
       </c>
       <c r="AM3">
-        <v>0</v>
+        <v>-179.9999999999404</v>
       </c>
       <c r="AN3">
-        <v>179.9999999999737</v>
+        <v>179.9999999999346</v>
       </c>
       <c r="AO3">
-        <v>2.263570042986083E-11</v>
+        <v>4.559487397231727E-13</v>
       </c>
       <c r="AP3">
-        <v>0</v>
+        <v>-179.9999999999257</v>
       </c>
       <c r="AQ3">
-        <v>179.999999999969</v>
+        <v>179.9999999999208</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -3473,22 +3473,22 @@
         <v>0.8660254037863299</v>
       </c>
       <c r="AL4">
-        <v>1.780692173543077E-11</v>
+        <v>5.344175747881745E-13</v>
       </c>
       <c r="AM4">
-        <v>0</v>
+        <v>-179.9999999999404</v>
       </c>
       <c r="AN4">
-        <v>179.9999999999737</v>
+        <v>179.9999999999346</v>
       </c>
       <c r="AO4">
-        <v>2.263853053768626E-11</v>
+        <v>4.347494640096741E-13</v>
       </c>
       <c r="AP4">
-        <v>0</v>
+        <v>-179.9999999999256</v>
       </c>
       <c r="AQ4">
-        <v>179.999999999969</v>
+        <v>179.9999999999208</v>
       </c>
     </row>
   </sheetData>
@@ -3748,22 +3748,22 @@
         <v>0.8245148352676808</v>
       </c>
       <c r="AL2">
-        <v>11.96551486068327</v>
+        <v>4.175225802073761E-13</v>
       </c>
       <c r="AM2">
-        <v>-113.1494187269337</v>
+        <v>-151.7090141414926</v>
       </c>
       <c r="AN2">
-        <v>165.4883827685514</v>
+        <v>135.0798105189271</v>
       </c>
       <c r="AO2">
-        <v>11.32964460932057</v>
+        <v>3.237023925379371E-13</v>
       </c>
       <c r="AP2">
-        <v>-108.6437575167419</v>
+        <v>-152.0992952265734</v>
       </c>
       <c r="AQ2">
-        <v>166.9558387682455</v>
+        <v>140.5172163445682</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -3879,22 +3879,22 @@
         <v>0.8378069029743125</v>
       </c>
       <c r="AL3">
-        <v>11.32964460932057</v>
+        <v>3.237023925379371E-13</v>
       </c>
       <c r="AM3">
-        <v>-108.6437575167419</v>
+        <v>-152.0992952265734</v>
       </c>
       <c r="AN3">
-        <v>166.9558387682455</v>
+        <v>140.5172163445682</v>
       </c>
       <c r="AO3">
-        <v>10.61318659607675</v>
+        <v>2.93753893670413E-13</v>
       </c>
       <c r="AP3">
-        <v>-105.013681139927</v>
+        <v>-152.9417769804534</v>
       </c>
       <c r="AQ3">
-        <v>168.2323053037849</v>
+        <v>144.8701151508106</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -4010,22 +4010,22 @@
         <v>0.8378069029743125</v>
       </c>
       <c r="AL4">
-        <v>11.32964460932057</v>
+        <v>3.237023925379371E-13</v>
       </c>
       <c r="AM4">
-        <v>-108.6437575167419</v>
+        <v>-152.0992952265734</v>
       </c>
       <c r="AN4">
-        <v>166.9558387682455</v>
+        <v>140.5172163445682</v>
       </c>
       <c r="AO4">
-        <v>10.61318659607676</v>
+        <v>2.815438472200884E-13</v>
       </c>
       <c r="AP4">
-        <v>-105.013681139927</v>
+        <v>-152.9417769804534</v>
       </c>
       <c r="AQ4">
-        <v>168.232305303785</v>
+        <v>144.8701151508107</v>
       </c>
     </row>
   </sheetData>
@@ -4285,22 +4285,22 @@
         <v>0.8245148352676808</v>
       </c>
       <c r="AL2">
-        <v>11.96551486068327</v>
+        <v>4.175225802073761E-13</v>
       </c>
       <c r="AM2">
-        <v>-113.1494187269337</v>
+        <v>-151.7090141414926</v>
       </c>
       <c r="AN2">
-        <v>165.4883827685514</v>
+        <v>135.0798105189271</v>
       </c>
       <c r="AO2">
-        <v>11.32964460932057</v>
+        <v>3.237023925379371E-13</v>
       </c>
       <c r="AP2">
-        <v>-108.6437575167419</v>
+        <v>-152.0992952265734</v>
       </c>
       <c r="AQ2">
-        <v>166.9558387682455</v>
+        <v>140.5172163445682</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -4416,22 +4416,22 @@
         <v>0.8378069029743125</v>
       </c>
       <c r="AL3">
-        <v>11.32964460932057</v>
+        <v>3.237023925379371E-13</v>
       </c>
       <c r="AM3">
-        <v>-108.6437575167419</v>
+        <v>-152.0992952265734</v>
       </c>
       <c r="AN3">
-        <v>166.9558387682455</v>
+        <v>140.5172163445682</v>
       </c>
       <c r="AO3">
-        <v>10.61318659607675</v>
+        <v>2.93753893670413E-13</v>
       </c>
       <c r="AP3">
-        <v>-105.013681139927</v>
+        <v>-152.9417769804534</v>
       </c>
       <c r="AQ3">
-        <v>168.2323053037849</v>
+        <v>144.8701151508106</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -4547,22 +4547,22 @@
         <v>0.8378069029743125</v>
       </c>
       <c r="AL4">
-        <v>11.32964460932057</v>
+        <v>3.237023925379371E-13</v>
       </c>
       <c r="AM4">
-        <v>-108.6437575167419</v>
+        <v>-152.0992952265734</v>
       </c>
       <c r="AN4">
-        <v>166.9558387682455</v>
+        <v>140.5172163445682</v>
       </c>
       <c r="AO4">
-        <v>10.61318659607676</v>
+        <v>2.815438472200884E-13</v>
       </c>
       <c r="AP4">
-        <v>-105.013681139927</v>
+        <v>-152.9417769804534</v>
       </c>
       <c r="AQ4">
-        <v>168.232305303785</v>
+        <v>144.8701151508107</v>
       </c>
     </row>
   </sheetData>
@@ -4822,22 +4822,22 @@
         <v>0.7178088852998012</v>
       </c>
       <c r="AL2">
-        <v>-0.01117384664767678</v>
+        <v>-0.01117384647240266</v>
       </c>
       <c r="AM2">
         <v>0</v>
       </c>
       <c r="AN2">
-        <v>179.9888261535143</v>
+        <v>0</v>
       </c>
       <c r="AO2">
-        <v>-6.313450644998808</v>
+        <v>-6.313450644914343</v>
       </c>
       <c r="AP2">
         <v>0</v>
       </c>
       <c r="AQ2">
-        <v>173.6865493550667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -4953,22 +4953,22 @@
         <v>0.7719945678096874</v>
       </c>
       <c r="AL3">
-        <v>-6.313450644998808</v>
+        <v>-6.313450644914343</v>
       </c>
       <c r="AM3">
         <v>0</v>
       </c>
       <c r="AN3">
-        <v>173.6865493550667</v>
+        <v>0</v>
       </c>
       <c r="AO3">
-        <v>-6.619958059522241</v>
+        <v>-6.619958059475713</v>
       </c>
       <c r="AP3">
         <v>0</v>
       </c>
       <c r="AQ3">
-        <v>173.3800419405132</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -5084,22 +5084,22 @@
         <v>0.7719945678096877</v>
       </c>
       <c r="AL4">
-        <v>-6.313450644998808</v>
+        <v>-6.313450644914343</v>
       </c>
       <c r="AM4">
         <v>0</v>
       </c>
       <c r="AN4">
-        <v>173.6865493550667</v>
+        <v>0</v>
       </c>
       <c r="AO4">
-        <v>-6.619958059522241</v>
+        <v>-6.619958059475715</v>
       </c>
       <c r="AP4">
         <v>0</v>
       </c>
       <c r="AQ4">
-        <v>173.3800419405131</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5359,22 +5359,22 @@
         <v>0.7178088852998012</v>
       </c>
       <c r="AL2">
-        <v>-0.01117384664767678</v>
+        <v>-0.01117384647240266</v>
       </c>
       <c r="AM2">
         <v>0</v>
       </c>
       <c r="AN2">
-        <v>179.9888261535143</v>
+        <v>0</v>
       </c>
       <c r="AO2">
-        <v>-6.313450644998808</v>
+        <v>-6.313450644914343</v>
       </c>
       <c r="AP2">
         <v>0</v>
       </c>
       <c r="AQ2">
-        <v>173.6865493550667</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -5490,22 +5490,22 @@
         <v>0.7719945678096874</v>
       </c>
       <c r="AL3">
-        <v>-6.313450644998808</v>
+        <v>-6.313450644914343</v>
       </c>
       <c r="AM3">
         <v>0</v>
       </c>
       <c r="AN3">
-        <v>173.6865493550667</v>
+        <v>0</v>
       </c>
       <c r="AO3">
-        <v>-6.619958059522241</v>
+        <v>-6.619958059475713</v>
       </c>
       <c r="AP3">
         <v>0</v>
       </c>
       <c r="AQ3">
-        <v>173.3800419405132</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -5621,22 +5621,22 @@
         <v>0.7719945678096877</v>
       </c>
       <c r="AL4">
-        <v>-6.313450644998808</v>
+        <v>-6.313450644914343</v>
       </c>
       <c r="AM4">
         <v>0</v>
       </c>
       <c r="AN4">
-        <v>173.6865493550667</v>
+        <v>0</v>
       </c>
       <c r="AO4">
-        <v>-6.619958059522241</v>
+        <v>-6.619958059475715</v>
       </c>
       <c r="AP4">
         <v>0</v>
       </c>
       <c r="AQ4">
-        <v>173.3800419405131</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -5896,22 +5896,22 @@
         <v>0.8518280946068217</v>
       </c>
       <c r="AL2">
-        <v>17.56327454668237</v>
+        <v>0.0139270167001685</v>
       </c>
       <c r="AM2">
-        <v>-104.8932091443124</v>
+        <v>-134.8639182893703</v>
       </c>
       <c r="AN2">
-        <v>151.7220699253674</v>
+        <v>105.0635730055186</v>
       </c>
       <c r="AO2">
-        <v>16.29079354750229</v>
+        <v>-2.700740752990738</v>
       </c>
       <c r="AP2">
-        <v>-104.1338952714761</v>
+        <v>-129.4216267706429</v>
       </c>
       <c r="AQ2">
-        <v>153.6019224867848</v>
+        <v>103.8229478846527</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -6027,22 +6027,22 @@
         <v>0.8564846443872474</v>
       </c>
       <c r="AL3">
-        <v>16.29079354750229</v>
+        <v>-2.700740752990738</v>
       </c>
       <c r="AM3">
-        <v>-104.1338952714761</v>
+        <v>-129.4216267706429</v>
       </c>
       <c r="AN3">
-        <v>153.6019224867848</v>
+        <v>103.8229478846527</v>
       </c>
       <c r="AO3">
-        <v>15.26462421738486</v>
+        <v>-3.782899000602696</v>
       </c>
       <c r="AP3">
-        <v>-103.4693739255812</v>
+        <v>-125.5778459566468</v>
       </c>
       <c r="AQ3">
-        <v>155.2583730680015</v>
+        <v>102.267677590504</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -6158,22 +6158,22 @@
         <v>0.8564846443872474</v>
       </c>
       <c r="AL4">
-        <v>16.29079354750229</v>
+        <v>-2.700740752990738</v>
       </c>
       <c r="AM4">
-        <v>-104.1338952714761</v>
+        <v>-129.4216267706429</v>
       </c>
       <c r="AN4">
-        <v>153.6019224867848</v>
+        <v>103.8229478846527</v>
       </c>
       <c r="AO4">
-        <v>15.26462421738487</v>
+        <v>-3.782899000602703</v>
       </c>
       <c r="AP4">
-        <v>-103.4693739255812</v>
+        <v>-125.5778459566467</v>
       </c>
       <c r="AQ4">
-        <v>155.2583730680015</v>
+        <v>102.267677590504</v>
       </c>
     </row>
   </sheetData>
@@ -6289,10 +6289,10 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>84.28940675037381</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>79.08778074434936</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -6342,10 +6342,10 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>79.08778074434936</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>75.11055707408345</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -6395,10 +6395,10 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>79.08778074434936</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>75.11055707408345</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -6658,22 +6658,22 @@
         <v>0.8518280946068217</v>
       </c>
       <c r="AL2">
-        <v>17.56327454668237</v>
+        <v>0.0139270167001685</v>
       </c>
       <c r="AM2">
-        <v>-104.8932091443124</v>
+        <v>-134.8639182893703</v>
       </c>
       <c r="AN2">
-        <v>151.7220699253674</v>
+        <v>105.0635730055186</v>
       </c>
       <c r="AO2">
-        <v>16.29079354750229</v>
+        <v>-2.700740752990738</v>
       </c>
       <c r="AP2">
-        <v>-104.1338952714761</v>
+        <v>-129.4216267706429</v>
       </c>
       <c r="AQ2">
-        <v>153.6019224867848</v>
+        <v>103.8229478846527</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -6789,22 +6789,22 @@
         <v>0.8564846443872474</v>
       </c>
       <c r="AL3">
-        <v>16.29079354750229</v>
+        <v>-2.700740752990738</v>
       </c>
       <c r="AM3">
-        <v>-104.1338952714761</v>
+        <v>-129.4216267706429</v>
       </c>
       <c r="AN3">
-        <v>153.6019224867848</v>
+        <v>103.8229478846527</v>
       </c>
       <c r="AO3">
-        <v>15.26462421738486</v>
+        <v>-3.782899000602696</v>
       </c>
       <c r="AP3">
-        <v>-103.4693739255812</v>
+        <v>-125.5778459566468</v>
       </c>
       <c r="AQ3">
-        <v>155.2583730680015</v>
+        <v>102.267677590504</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -6920,22 +6920,22 @@
         <v>0.8564846443872474</v>
       </c>
       <c r="AL4">
-        <v>16.29079354750229</v>
+        <v>-2.700740752990738</v>
       </c>
       <c r="AM4">
-        <v>-104.1338952714761</v>
+        <v>-129.4216267706429</v>
       </c>
       <c r="AN4">
-        <v>153.6019224867848</v>
+        <v>103.8229478846527</v>
       </c>
       <c r="AO4">
-        <v>15.26462421738487</v>
+        <v>-3.782899000602703</v>
       </c>
       <c r="AP4">
-        <v>-103.4693739255812</v>
+        <v>-125.5778459566467</v>
       </c>
       <c r="AQ4">
-        <v>155.2583730680015</v>
+        <v>102.267677590504</v>
       </c>
     </row>
   </sheetData>
@@ -7195,22 +7195,22 @@
         <v>0.6950234972340121</v>
       </c>
       <c r="AL2">
-        <v>-0.01310313119137088</v>
+        <v>-0.01310313133982031</v>
       </c>
       <c r="AM2">
         <v>0</v>
       </c>
       <c r="AN2">
-        <v>179.9868968685288</v>
+        <v>0</v>
       </c>
       <c r="AO2">
-        <v>-7.611827049086783</v>
+        <v>-7.611827049154744</v>
       </c>
       <c r="AP2">
         <v>0</v>
       </c>
       <c r="AQ2">
-        <v>172.3881729507654</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -7326,22 +7326,22 @@
         <v>0.7474500608986431</v>
       </c>
       <c r="AL3">
-        <v>-7.611827049086783</v>
+        <v>-7.611827049154744</v>
       </c>
       <c r="AM3">
         <v>0</v>
       </c>
       <c r="AN3">
-        <v>172.3881729507654</v>
+        <v>0</v>
       </c>
       <c r="AO3">
-        <v>-6.297561754805892</v>
+        <v>-6.297561754845085</v>
       </c>
       <c r="AP3">
         <v>0</v>
       </c>
       <c r="AQ3">
-        <v>173.702438245086</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -7457,22 +7457,22 @@
         <v>0.7474500608986436</v>
       </c>
       <c r="AL4">
-        <v>-7.611827049086783</v>
+        <v>-7.611827049154744</v>
       </c>
       <c r="AM4">
         <v>0</v>
       </c>
       <c r="AN4">
-        <v>172.3881729507654</v>
+        <v>0</v>
       </c>
       <c r="AO4">
-        <v>-6.297561754805924</v>
+        <v>-6.29756175484508</v>
       </c>
       <c r="AP4">
         <v>0</v>
       </c>
       <c r="AQ4">
-        <v>173.702438245086</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -7732,22 +7732,22 @@
         <v>0.6950234972340121</v>
       </c>
       <c r="AL2">
-        <v>-0.01310313119137088</v>
+        <v>-0.01310313133982031</v>
       </c>
       <c r="AM2">
         <v>0</v>
       </c>
       <c r="AN2">
-        <v>179.9868968685288</v>
+        <v>0</v>
       </c>
       <c r="AO2">
-        <v>-7.611827049086783</v>
+        <v>-7.611827049154744</v>
       </c>
       <c r="AP2">
         <v>0</v>
       </c>
       <c r="AQ2">
-        <v>172.3881729507654</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -7863,22 +7863,22 @@
         <v>0.7474500608986431</v>
       </c>
       <c r="AL3">
-        <v>-7.611827049086783</v>
+        <v>-7.611827049154744</v>
       </c>
       <c r="AM3">
         <v>0</v>
       </c>
       <c r="AN3">
-        <v>172.3881729507654</v>
+        <v>0</v>
       </c>
       <c r="AO3">
-        <v>-6.297561754805892</v>
+        <v>-6.297561754845085</v>
       </c>
       <c r="AP3">
         <v>0</v>
       </c>
       <c r="AQ3">
-        <v>173.702438245086</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -7994,22 +7994,22 @@
         <v>0.7474500608986436</v>
       </c>
       <c r="AL4">
-        <v>-7.611827049086783</v>
+        <v>-7.611827049154744</v>
       </c>
       <c r="AM4">
         <v>0</v>
       </c>
       <c r="AN4">
-        <v>172.3881729507654</v>
+        <v>0</v>
       </c>
       <c r="AO4">
-        <v>-6.297561754805924</v>
+        <v>-6.29756175484508</v>
       </c>
       <c r="AP4">
         <v>0</v>
       </c>
       <c r="AQ4">
-        <v>173.702438245086</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8269,22 +8269,22 @@
         <v>0.7780446838807024</v>
       </c>
       <c r="AL2">
-        <v>16.55576890986408</v>
+        <v>0.0158194676764636</v>
       </c>
       <c r="AM2">
-        <v>-106.1399873258002</v>
+        <v>-136.1029564689277</v>
       </c>
       <c r="AN2">
-        <v>152.3303371030605</v>
+        <v>103.8071623873661</v>
       </c>
       <c r="AO2">
-        <v>15.07716951670869</v>
+        <v>-4.351556157237489</v>
       </c>
       <c r="AP2">
-        <v>-103.4150584572222</v>
+        <v>-125.9235815556908</v>
       </c>
       <c r="AQ2">
-        <v>154.9843720112472</v>
+        <v>103.3157265540677</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -8400,22 +8400,22 @@
         <v>0.793440478635774</v>
       </c>
       <c r="AL3">
-        <v>15.07716951670869</v>
+        <v>-4.351556157237489</v>
       </c>
       <c r="AM3">
-        <v>-103.4150584572222</v>
+        <v>-125.9235815556908</v>
       </c>
       <c r="AN3">
-        <v>154.9843720112472</v>
+        <v>103.3157265540677</v>
       </c>
       <c r="AO3">
-        <v>14.16121021104031</v>
+        <v>-5.054191003316187</v>
       </c>
       <c r="AP3">
-        <v>-101.1058570224848</v>
+        <v>-119.3656480962875</v>
       </c>
       <c r="AQ3">
-        <v>157.3127817016637</v>
+        <v>101.6931454031112</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -8531,22 +8531,22 @@
         <v>0.793440478635774</v>
       </c>
       <c r="AL4">
-        <v>15.07716951670869</v>
+        <v>-4.351556157237489</v>
       </c>
       <c r="AM4">
-        <v>-103.4150584572222</v>
+        <v>-125.9235815556908</v>
       </c>
       <c r="AN4">
-        <v>154.9843720112472</v>
+        <v>103.3157265540677</v>
       </c>
       <c r="AO4">
-        <v>14.1612102110403</v>
+        <v>-5.054191003316185</v>
       </c>
       <c r="AP4">
-        <v>-101.1058570224848</v>
+        <v>-119.3656480962875</v>
       </c>
       <c r="AQ4">
-        <v>157.3127817016637</v>
+        <v>101.6931454031111</v>
       </c>
     </row>
   </sheetData>
@@ -8806,22 +8806,22 @@
         <v>0.7780446838807024</v>
       </c>
       <c r="AL2">
-        <v>16.55576890986408</v>
+        <v>0.0158194676764636</v>
       </c>
       <c r="AM2">
-        <v>-106.1399873258002</v>
+        <v>-136.1029564689277</v>
       </c>
       <c r="AN2">
-        <v>152.3303371030605</v>
+        <v>103.8071623873661</v>
       </c>
       <c r="AO2">
-        <v>15.07716951670869</v>
+        <v>-4.351556157237489</v>
       </c>
       <c r="AP2">
-        <v>-103.4150584572222</v>
+        <v>-125.9235815556908</v>
       </c>
       <c r="AQ2">
-        <v>154.9843720112472</v>
+        <v>103.3157265540677</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -8937,22 +8937,22 @@
         <v>0.793440478635774</v>
       </c>
       <c r="AL3">
-        <v>15.07716951670869</v>
+        <v>-4.351556157237489</v>
       </c>
       <c r="AM3">
-        <v>-103.4150584572222</v>
+        <v>-125.9235815556908</v>
       </c>
       <c r="AN3">
-        <v>154.9843720112472</v>
+        <v>103.3157265540677</v>
       </c>
       <c r="AO3">
-        <v>14.16121021104031</v>
+        <v>-5.054191003316187</v>
       </c>
       <c r="AP3">
-        <v>-101.1058570224848</v>
+        <v>-119.3656480962875</v>
       </c>
       <c r="AQ3">
-        <v>157.3127817016637</v>
+        <v>101.6931454031112</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -9068,22 +9068,22 @@
         <v>0.793440478635774</v>
       </c>
       <c r="AL4">
-        <v>15.07716951670869</v>
+        <v>-4.351556157237489</v>
       </c>
       <c r="AM4">
-        <v>-103.4150584572222</v>
+        <v>-125.9235815556908</v>
       </c>
       <c r="AN4">
-        <v>154.9843720112472</v>
+        <v>103.3157265540677</v>
       </c>
       <c r="AO4">
-        <v>14.1612102110403</v>
+        <v>-5.054191003316185</v>
       </c>
       <c r="AP4">
-        <v>-101.1058570224848</v>
+        <v>-119.3656480962875</v>
       </c>
       <c r="AQ4">
-        <v>157.3127817016637</v>
+        <v>101.6931454031111</v>
       </c>
     </row>
   </sheetData>
@@ -9343,22 +9343,22 @@
         <v>0.7599982922815229</v>
       </c>
       <c r="AL2">
-        <v>59.90088731360098</v>
+        <v>0</v>
       </c>
       <c r="AM2">
-        <v>-89.99999999999633</v>
+        <v>-120.0991126865173</v>
       </c>
       <c r="AN2">
-        <v>120.0878544346237</v>
+        <v>120.0878544348442</v>
       </c>
       <c r="AO2">
-        <v>48.84809195671546</v>
+        <v>0</v>
       </c>
       <c r="AP2">
-        <v>-89.99999999999643</v>
+        <v>-131.1519080433461</v>
       </c>
       <c r="AQ2">
-        <v>121.109045449341</v>
+        <v>121.1090454494766</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -9474,22 +9474,22 @@
         <v>0.826836754355374</v>
       </c>
       <c r="AL3">
-        <v>48.84809195671546</v>
+        <v>0</v>
       </c>
       <c r="AM3">
-        <v>-89.99999999999643</v>
+        <v>-131.1519080433461</v>
       </c>
       <c r="AN3">
-        <v>121.109045449341</v>
+        <v>121.1090454494766</v>
       </c>
       <c r="AO3">
-        <v>41.92164926482276</v>
+        <v>0</v>
       </c>
       <c r="AP3">
-        <v>-89.9999999999964</v>
+        <v>-138.0783507352045</v>
       </c>
       <c r="AQ3">
-        <v>123.7614475143174</v>
+        <v>123.7614475144085</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -9605,22 +9605,22 @@
         <v>0.8268367543553737</v>
       </c>
       <c r="AL4">
-        <v>48.84809195671546</v>
+        <v>0</v>
       </c>
       <c r="AM4">
-        <v>-89.99999999999643</v>
+        <v>-131.1519080433461</v>
       </c>
       <c r="AN4">
-        <v>121.109045449341</v>
+        <v>121.1090454494766</v>
       </c>
       <c r="AO4">
-        <v>41.92164926482278</v>
+        <v>0</v>
       </c>
       <c r="AP4">
-        <v>-89.99999999999639</v>
+        <v>-138.0783507352045</v>
       </c>
       <c r="AQ4">
-        <v>123.7614475143174</v>
+        <v>123.7614475144085</v>
       </c>
     </row>
   </sheetData>
@@ -9880,22 +9880,22 @@
         <v>0.7599982922815229</v>
       </c>
       <c r="AL2">
-        <v>59.90088731360098</v>
+        <v>0</v>
       </c>
       <c r="AM2">
-        <v>-89.99999999999633</v>
+        <v>-120.0991126865173</v>
       </c>
       <c r="AN2">
-        <v>120.0878544346237</v>
+        <v>120.0878544348442</v>
       </c>
       <c r="AO2">
-        <v>48.84809195671546</v>
+        <v>0</v>
       </c>
       <c r="AP2">
-        <v>-89.99999999999643</v>
+        <v>-131.1519080433461</v>
       </c>
       <c r="AQ2">
-        <v>121.109045449341</v>
+        <v>121.1090454494766</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -10011,22 +10011,22 @@
         <v>0.826836754355374</v>
       </c>
       <c r="AL3">
-        <v>48.84809195671546</v>
+        <v>0</v>
       </c>
       <c r="AM3">
-        <v>-89.99999999999643</v>
+        <v>-131.1519080433461</v>
       </c>
       <c r="AN3">
-        <v>121.109045449341</v>
+        <v>121.1090454494766</v>
       </c>
       <c r="AO3">
-        <v>41.92164926482276</v>
+        <v>0</v>
       </c>
       <c r="AP3">
-        <v>-89.9999999999964</v>
+        <v>-138.0783507352045</v>
       </c>
       <c r="AQ3">
-        <v>123.7614475143174</v>
+        <v>123.7614475144085</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -10142,22 +10142,22 @@
         <v>0.8268367543553737</v>
       </c>
       <c r="AL4">
-        <v>48.84809195671546</v>
+        <v>0</v>
       </c>
       <c r="AM4">
-        <v>-89.99999999999643</v>
+        <v>-131.1519080433461</v>
       </c>
       <c r="AN4">
-        <v>121.109045449341</v>
+        <v>121.1090454494766</v>
       </c>
       <c r="AO4">
-        <v>41.92164926482278</v>
+        <v>0</v>
       </c>
       <c r="AP4">
-        <v>-89.99999999999639</v>
+        <v>-138.0783507352045</v>
       </c>
       <c r="AQ4">
-        <v>123.7614475143174</v>
+        <v>123.7614475144085</v>
       </c>
     </row>
   </sheetData>
@@ -10417,22 +10417,22 @@
         <v>0.9689144874145577</v>
       </c>
       <c r="AL2">
-        <v>31.7119228523478</v>
+        <v>-14.90717692343631</v>
       </c>
       <c r="AM2">
-        <v>-89.99999999999653</v>
+        <v>-120.0292704737576</v>
       </c>
       <c r="AN2">
-        <v>137.5699449588465</v>
+        <v>120.0432382313321</v>
       </c>
       <c r="AO2">
-        <v>31.98508613615191</v>
+        <v>-10.59028714735436</v>
       </c>
       <c r="AP2">
-        <v>-89.99999999999645</v>
+        <v>-125.1315647199126</v>
       </c>
       <c r="AQ2">
-        <v>137.6328508700616</v>
+        <v>121.6238606247693</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -10548,22 +10548,22 @@
         <v>0.9656494086163243</v>
       </c>
       <c r="AL3">
-        <v>31.98508613615191</v>
+        <v>-10.59028714735436</v>
       </c>
       <c r="AM3">
-        <v>-89.99999999999645</v>
+        <v>-125.1315647199126</v>
       </c>
       <c r="AN3">
-        <v>137.6328508700616</v>
+        <v>121.6238606247693</v>
       </c>
       <c r="AO3">
-        <v>32.20512181945389</v>
+        <v>-7.303623184977604</v>
       </c>
       <c r="AP3">
-        <v>-89.9999999999964</v>
+        <v>-129.0553880005655</v>
       </c>
       <c r="AQ3">
-        <v>137.6537678120567</v>
+        <v>123.0990884522615</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -10679,22 +10679,22 @@
         <v>0.9656494086163243</v>
       </c>
       <c r="AL4">
-        <v>31.98508613615191</v>
+        <v>-10.59028714735436</v>
       </c>
       <c r="AM4">
-        <v>-89.99999999999645</v>
+        <v>-125.1315647199126</v>
       </c>
       <c r="AN4">
-        <v>137.6328508700616</v>
+        <v>121.6238606247693</v>
       </c>
       <c r="AO4">
-        <v>32.20512181945389</v>
+        <v>-7.303623184977599</v>
       </c>
       <c r="AP4">
-        <v>-89.9999999999964</v>
+        <v>-129.0553880005655</v>
       </c>
       <c r="AQ4">
-        <v>137.6537678120567</v>
+        <v>123.0990884522615</v>
       </c>
     </row>
   </sheetData>
@@ -10954,22 +10954,22 @@
         <v>0.9689144874145577</v>
       </c>
       <c r="AL2">
-        <v>31.7119228523478</v>
+        <v>-14.90717692343631</v>
       </c>
       <c r="AM2">
-        <v>-89.99999999999653</v>
+        <v>-120.0292704737576</v>
       </c>
       <c r="AN2">
-        <v>137.5699449588465</v>
+        <v>120.0432382313321</v>
       </c>
       <c r="AO2">
-        <v>31.98508613615191</v>
+        <v>-10.59028714735436</v>
       </c>
       <c r="AP2">
-        <v>-89.99999999999645</v>
+        <v>-125.1315647199126</v>
       </c>
       <c r="AQ2">
-        <v>137.6328508700616</v>
+        <v>121.6238606247693</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -11085,22 +11085,22 @@
         <v>0.9656494086163243</v>
       </c>
       <c r="AL3">
-        <v>31.98508613615191</v>
+        <v>-10.59028714735436</v>
       </c>
       <c r="AM3">
-        <v>-89.99999999999645</v>
+        <v>-125.1315647199126</v>
       </c>
       <c r="AN3">
-        <v>137.6328508700616</v>
+        <v>121.6238606247693</v>
       </c>
       <c r="AO3">
-        <v>32.20512181945389</v>
+        <v>-7.303623184977604</v>
       </c>
       <c r="AP3">
-        <v>-89.9999999999964</v>
+        <v>-129.0553880005655</v>
       </c>
       <c r="AQ3">
-        <v>137.6537678120567</v>
+        <v>123.0990884522615</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -11216,22 +11216,22 @@
         <v>0.9656494086163243</v>
       </c>
       <c r="AL4">
-        <v>31.98508613615191</v>
+        <v>-10.59028714735436</v>
       </c>
       <c r="AM4">
-        <v>-89.99999999999645</v>
+        <v>-125.1315647199126</v>
       </c>
       <c r="AN4">
-        <v>137.6328508700616</v>
+        <v>121.6238606247693</v>
       </c>
       <c r="AO4">
-        <v>32.20512181945389</v>
+        <v>-7.303623184977599</v>
       </c>
       <c r="AP4">
-        <v>-89.9999999999964</v>
+        <v>-129.0553880005655</v>
       </c>
       <c r="AQ4">
-        <v>137.6537678120567</v>
+        <v>123.0990884522615</v>
       </c>
     </row>
   </sheetData>
@@ -11491,22 +11491,22 @@
         <v>0.7514492206972073</v>
       </c>
       <c r="AL2">
-        <v>59.88716006626888</v>
+        <v>0</v>
       </c>
       <c r="AM2">
-        <v>-89.99999999999636</v>
+        <v>-120.1128399339563</v>
       </c>
       <c r="AN2">
-        <v>120.0996242896476</v>
+        <v>120.0996242898029</v>
       </c>
       <c r="AO2">
-        <v>42.2903649473445</v>
+        <v>0</v>
       </c>
       <c r="AP2">
-        <v>-89.99999999999652</v>
+        <v>-137.7096350527863</v>
       </c>
       <c r="AQ2">
-        <v>122.1643601284607</v>
+        <v>122.1643601285336</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -11622,22 +11622,22 @@
         <v>0.8180273553921663</v>
       </c>
       <c r="AL3">
-        <v>42.2903649473445</v>
+        <v>0</v>
       </c>
       <c r="AM3">
-        <v>-89.99999999999652</v>
+        <v>-137.7096350527863</v>
       </c>
       <c r="AN3">
-        <v>122.1643601284607</v>
+        <v>122.1643601285336</v>
       </c>
       <c r="AO3">
-        <v>35.14600558028982</v>
+        <v>0</v>
       </c>
       <c r="AP3">
-        <v>-89.99999999999639</v>
+        <v>-144.8539944197721</v>
       </c>
       <c r="AQ3">
-        <v>126.7970300907754</v>
+        <v>126.7970300908124</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -11753,22 +11753,22 @@
         <v>0.8180273553921662</v>
       </c>
       <c r="AL4">
-        <v>42.2903649473445</v>
+        <v>0</v>
       </c>
       <c r="AM4">
-        <v>-89.99999999999652</v>
+        <v>-137.7096350527863</v>
       </c>
       <c r="AN4">
-        <v>122.1643601284607</v>
+        <v>122.1643601285336</v>
       </c>
       <c r="AO4">
-        <v>35.14600558028984</v>
+        <v>0</v>
       </c>
       <c r="AP4">
-        <v>-89.99999999999639</v>
+        <v>-144.8539944197721</v>
       </c>
       <c r="AQ4">
-        <v>126.7970300907753</v>
+        <v>126.7970300908124</v>
       </c>
     </row>
   </sheetData>
@@ -11884,10 +11884,10 @@
         <v>0.6697864322467405</v>
       </c>
       <c r="P2">
-        <v>45.00000000003757</v>
+        <v>-14.89320914423961</v>
       </c>
       <c r="Q2">
-        <v>45.00000000003514</v>
+        <v>-14.13389527141264</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -11937,10 +11937,10 @@
         <v>0.627932206981674</v>
       </c>
       <c r="P3">
-        <v>45.00000000003514</v>
+        <v>-14.13389527141264</v>
       </c>
       <c r="Q3">
-        <v>45.000000000033</v>
+        <v>-13.46937392552527</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -11990,10 +11990,10 @@
         <v>0.6279322069816738</v>
       </c>
       <c r="P4">
-        <v>45.00000000003514</v>
+        <v>-14.13389527141264</v>
       </c>
       <c r="Q4">
-        <v>45.00000000003298</v>
+        <v>-13.46937392552528</v>
       </c>
     </row>
   </sheetData>
@@ -12253,22 +12253,22 @@
         <v>0.7514492206972073</v>
       </c>
       <c r="AL2">
-        <v>59.88716006626888</v>
+        <v>0</v>
       </c>
       <c r="AM2">
-        <v>-89.99999999999636</v>
+        <v>-120.1128399339563</v>
       </c>
       <c r="AN2">
-        <v>120.0996242896476</v>
+        <v>120.0996242898029</v>
       </c>
       <c r="AO2">
-        <v>42.2903649473445</v>
+        <v>0</v>
       </c>
       <c r="AP2">
-        <v>-89.99999999999652</v>
+        <v>-137.7096350527863</v>
       </c>
       <c r="AQ2">
-        <v>122.1643601284607</v>
+        <v>122.1643601285336</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -12384,22 +12384,22 @@
         <v>0.8180273553921663</v>
       </c>
       <c r="AL3">
-        <v>42.2903649473445</v>
+        <v>0</v>
       </c>
       <c r="AM3">
-        <v>-89.99999999999652</v>
+        <v>-137.7096350527863</v>
       </c>
       <c r="AN3">
-        <v>122.1643601284607</v>
+        <v>122.1643601285336</v>
       </c>
       <c r="AO3">
-        <v>35.14600558028982</v>
+        <v>0</v>
       </c>
       <c r="AP3">
-        <v>-89.99999999999639</v>
+        <v>-144.8539944197721</v>
       </c>
       <c r="AQ3">
-        <v>126.7970300907754</v>
+        <v>126.7970300908124</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -12515,22 +12515,22 @@
         <v>0.8180273553921662</v>
       </c>
       <c r="AL4">
-        <v>42.2903649473445</v>
+        <v>0</v>
       </c>
       <c r="AM4">
-        <v>-89.99999999999652</v>
+        <v>-137.7096350527863</v>
       </c>
       <c r="AN4">
-        <v>122.1643601284607</v>
+        <v>122.1643601285336</v>
       </c>
       <c r="AO4">
-        <v>35.14600558028984</v>
+        <v>0</v>
       </c>
       <c r="AP4">
-        <v>-89.99999999999639</v>
+        <v>-144.8539944197721</v>
       </c>
       <c r="AQ4">
-        <v>126.7970300907753</v>
+        <v>126.7970300908124</v>
       </c>
     </row>
   </sheetData>
@@ -12790,22 +12790,22 @@
         <v>0.877371251159636</v>
       </c>
       <c r="AL2">
-        <v>32.31584613269226</v>
+        <v>-16.15586420839396</v>
       </c>
       <c r="AM2">
-        <v>-89.99999999999655</v>
+        <v>-120.037002149499</v>
       </c>
       <c r="AN2">
-        <v>136.5651455806771</v>
+        <v>120.0528789941859</v>
       </c>
       <c r="AO2">
-        <v>32.13594383429049</v>
+        <v>-6.728172615731542</v>
       </c>
       <c r="AP2">
-        <v>-89.99999999999645</v>
+        <v>-128.6498735956027</v>
       </c>
       <c r="AQ2">
-        <v>137.3083573823813</v>
+        <v>122.1108182946456</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -12921,22 +12921,22 @@
         <v>0.8785874061674938</v>
       </c>
       <c r="AL3">
-        <v>32.13594383429049</v>
+        <v>-6.728172615731542</v>
       </c>
       <c r="AM3">
-        <v>-89.99999999999645</v>
+        <v>-128.6498735956027</v>
       </c>
       <c r="AN3">
-        <v>137.3083573823813</v>
+        <v>122.1108182946456</v>
       </c>
       <c r="AO3">
-        <v>32.21715262800947</v>
+        <v>-0.3048353219359057</v>
       </c>
       <c r="AP3">
-        <v>-89.99999999999638</v>
+        <v>-134.4515915409578</v>
       </c>
       <c r="AQ3">
-        <v>137.8628958470784</v>
+        <v>124.489614959663</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -13052,22 +13052,22 @@
         <v>0.8785874061674938</v>
       </c>
       <c r="AL4">
-        <v>32.13594383429049</v>
+        <v>-6.728172615731542</v>
       </c>
       <c r="AM4">
-        <v>-89.99999999999645</v>
+        <v>-128.6498735956027</v>
       </c>
       <c r="AN4">
-        <v>137.3083573823813</v>
+        <v>122.1108182946456</v>
       </c>
       <c r="AO4">
-        <v>32.21715262800947</v>
+        <v>-0.3048353219359008</v>
       </c>
       <c r="AP4">
-        <v>-89.99999999999636</v>
+        <v>-134.4515915409578</v>
       </c>
       <c r="AQ4">
-        <v>137.8628958470784</v>
+        <v>124.489614959663</v>
       </c>
     </row>
   </sheetData>
@@ -13327,22 +13327,22 @@
         <v>0.877371251159636</v>
       </c>
       <c r="AL2">
-        <v>32.31584613269226</v>
+        <v>-16.15586420839396</v>
       </c>
       <c r="AM2">
-        <v>-89.99999999999655</v>
+        <v>-120.037002149499</v>
       </c>
       <c r="AN2">
-        <v>136.5651455806771</v>
+        <v>120.0528789941859</v>
       </c>
       <c r="AO2">
-        <v>32.13594383429049</v>
+        <v>-6.728172615731542</v>
       </c>
       <c r="AP2">
-        <v>-89.99999999999645</v>
+        <v>-128.6498735956027</v>
       </c>
       <c r="AQ2">
-        <v>137.3083573823813</v>
+        <v>122.1108182946456</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -13458,22 +13458,22 @@
         <v>0.8785874061674938</v>
       </c>
       <c r="AL3">
-        <v>32.13594383429049</v>
+        <v>-6.728172615731542</v>
       </c>
       <c r="AM3">
-        <v>-89.99999999999645</v>
+        <v>-128.6498735956027</v>
       </c>
       <c r="AN3">
-        <v>137.3083573823813</v>
+        <v>122.1108182946456</v>
       </c>
       <c r="AO3">
-        <v>32.21715262800947</v>
+        <v>-0.3048353219359057</v>
       </c>
       <c r="AP3">
-        <v>-89.99999999999638</v>
+        <v>-134.4515915409578</v>
       </c>
       <c r="AQ3">
-        <v>137.8628958470784</v>
+        <v>124.489614959663</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -13589,22 +13589,22 @@
         <v>0.8785874061674938</v>
       </c>
       <c r="AL4">
-        <v>32.13594383429049</v>
+        <v>-6.728172615731542</v>
       </c>
       <c r="AM4">
-        <v>-89.99999999999645</v>
+        <v>-128.6498735956027</v>
       </c>
       <c r="AN4">
-        <v>137.3083573823813</v>
+        <v>122.1108182946456</v>
       </c>
       <c r="AO4">
-        <v>32.21715262800947</v>
+        <v>-0.3048353219359008</v>
       </c>
       <c r="AP4">
-        <v>-89.99999999999636</v>
+        <v>-134.4515915409578</v>
       </c>
       <c r="AQ4">
-        <v>137.8628958470784</v>
+        <v>124.489614959663</v>
       </c>
     </row>
   </sheetData>
@@ -13720,10 +13720,10 @@
         <v>0.6697864322467405</v>
       </c>
       <c r="P2">
-        <v>45.00000000003757</v>
+        <v>-14.89320914423961</v>
       </c>
       <c r="Q2">
-        <v>45.00000000003514</v>
+        <v>-14.13389527141264</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -13773,10 +13773,10 @@
         <v>0.627932206981674</v>
       </c>
       <c r="P3">
-        <v>45.00000000003514</v>
+        <v>-14.13389527141264</v>
       </c>
       <c r="Q3">
-        <v>45.000000000033</v>
+        <v>-13.46937392552527</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -13826,10 +13826,10 @@
         <v>0.6279322069816738</v>
       </c>
       <c r="P4">
-        <v>45.00000000003514</v>
+        <v>-14.13389527141264</v>
       </c>
       <c r="Q4">
-        <v>45.00000000003298</v>
+        <v>-13.46937392552528</v>
       </c>
     </row>
   </sheetData>
@@ -13945,10 +13945,10 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>84.28940674684127</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>74.95455943352283</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -13998,10 +13998,10 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>74.95455943352283</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>67.94031102776448</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -14051,10 +14051,10 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>74.95455943352283</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>67.94031102776448</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -14170,10 +14170,10 @@
         <v>0</v>
       </c>
       <c r="P2">
-        <v>84.28940674684127</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>74.95455943352283</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -14223,10 +14223,10 @@
         <v>0</v>
       </c>
       <c r="P3">
-        <v>74.95455943352283</v>
+        <v>0</v>
       </c>
       <c r="Q3">
-        <v>67.94031102776448</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -14276,10 +14276,10 @@
         <v>0</v>
       </c>
       <c r="P4">
-        <v>74.95455943352283</v>
+        <v>0</v>
       </c>
       <c r="Q4">
-        <v>67.94031102776448</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -14395,10 +14395,10 @@
         <v>0.5701359740005393</v>
       </c>
       <c r="P2">
-        <v>45.000000000111</v>
+        <v>-16.13998732580944</v>
       </c>
       <c r="Q2">
-        <v>45.00000000011345</v>
+        <v>-13.41505845719961</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -14448,10 +14448,10 @@
         <v>0.5261657129485261</v>
       </c>
       <c r="P3">
-        <v>45.00000000011345</v>
+        <v>-13.41505845719961</v>
       </c>
       <c r="Q3">
-        <v>45.00000000011481</v>
+        <v>-11.10585702243908</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -14501,10 +14501,10 @@
         <v>0.526165712948526</v>
       </c>
       <c r="P4">
-        <v>45.00000000011345</v>
+        <v>-13.41505845719961</v>
       </c>
       <c r="Q4">
-        <v>45.00000000011482</v>
+        <v>-11.10585702243908</v>
       </c>
     </row>
   </sheetData>
@@ -14620,10 +14620,10 @@
         <v>0.5701359740005393</v>
       </c>
       <c r="P2">
-        <v>45.000000000111</v>
+        <v>-16.13998732580944</v>
       </c>
       <c r="Q2">
-        <v>45.00000000011345</v>
+        <v>-13.41505845719961</v>
       </c>
     </row>
     <row r="3" spans="1:17">
@@ -14673,10 +14673,10 @@
         <v>0.5261657129485261</v>
       </c>
       <c r="P3">
-        <v>45.00000000011345</v>
+        <v>-13.41505845719961</v>
       </c>
       <c r="Q3">
-        <v>45.00000000011481</v>
+        <v>-11.10585702243908</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -14726,10 +14726,10 @@
         <v>0.526165712948526</v>
       </c>
       <c r="P4">
-        <v>45.00000000011345</v>
+        <v>-13.41505845719961</v>
       </c>
       <c r="Q4">
-        <v>45.00000000011482</v>
+        <v>-11.10585702243908</v>
       </c>
     </row>
   </sheetData>
@@ -14989,22 +14989,22 @@
         <v>0.952627964809529</v>
       </c>
       <c r="AL2">
-        <v>-6.289991047015337E-13</v>
+        <v>7.393038743051484E-13</v>
       </c>
       <c r="AM2">
-        <v>0</v>
+        <v>179.9999999999893</v>
       </c>
       <c r="AN2">
-        <v>179.9999999999919</v>
+        <v>179.9999999999889</v>
       </c>
       <c r="AO2">
-        <v>-4.852401742958505E-13</v>
+        <v>6.542352883650259E-13</v>
       </c>
       <c r="AP2">
-        <v>0</v>
+        <v>179.9999999999899</v>
       </c>
       <c r="AQ2">
-        <v>179.999999999992</v>
+        <v>179.9999999999892</v>
       </c>
     </row>
     <row r="3" spans="1:43">
@@ -15120,22 +15120,22 @@
         <v>0.9526279648097039</v>
       </c>
       <c r="AL3">
-        <v>-4.852401742958505E-13</v>
+        <v>6.542352883650259E-13</v>
       </c>
       <c r="AM3">
-        <v>0</v>
+        <v>179.9999999999899</v>
       </c>
       <c r="AN3">
-        <v>179.999999999992</v>
+        <v>179.9999999999892</v>
       </c>
       <c r="AO3">
-        <v>-3.643686092319228E-13</v>
+        <v>5.868810935265246E-13</v>
       </c>
       <c r="AP3">
-        <v>0</v>
+        <v>179.9999999999904</v>
       </c>
       <c r="AQ3">
-        <v>179.999999999992</v>
+        <v>179.9999999999894</v>
       </c>
     </row>
     <row r="4" spans="1:43">
@@ -15251,22 +15251,22 @@
         <v>0.9526279648097039</v>
       </c>
       <c r="AL4">
-        <v>-4.852401742958505E-13</v>
+        <v>6.542352883650259E-13</v>
       </c>
       <c r="AM4">
-        <v>0</v>
+        <v>179.9999999999899</v>
       </c>
       <c r="AN4">
-        <v>179.999999999992</v>
+        <v>179.9999999999892</v>
       </c>
       <c r="AO4">
-        <v>-3.588354961759716E-13</v>
+        <v>5.720494568375048E-13</v>
       </c>
       <c r="AP4">
-        <v>0</v>
+        <v>179.9999999999905</v>
       </c>
       <c r="AQ4">
-        <v>179.999999999992</v>
+        <v>179.9999999999895</v>
       </c>
     </row>
   </sheetData>

</xml_diff>